<commit_message>
Updated Working_Estimator_Script to be more efficient, added datetime column to data, updated game plan
</commit_message>
<xml_diff>
--- a/clean_df.xlsx
+++ b/clean_df.xlsx
@@ -1,30 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kijah\Documents\Data_Bootcamp\Estimator_Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99A2140-FF3B-4654-81DC-BDCEC5993B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="86">
   <si>
-    <t>Material Description</t>
-  </si>
-  <si>
-    <t>Material Price</t>
-  </si>
-  <si>
-    <t>Vendor Location</t>
-  </si>
-  <si>
     <t>link</t>
   </si>
   <si>
@@ -272,13 +269,22 @@
   </si>
   <si>
     <t>https://www.cooper-electric.com/product/detail/23760/thhn-copper-wic-thhn-10-str-blk-500r</t>
+  </si>
+  <si>
+    <t>Vendor_Location</t>
+  </si>
+  <si>
+    <t>Material_Price</t>
+  </si>
+  <si>
+    <t>Material_Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +360,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -400,7 +414,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -432,9 +446,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -466,6 +498,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -641,794 +691,800 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="64.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="119.1328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>7.22</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>5.99</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>4.73</v>
+        <v>4.7300000000000004</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>5.88</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>9.09</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>11.91</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>10.47</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>8.359999999999999</v>
+        <v>8.36</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>20.62</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>17.55</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>8.9</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>24.99</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>3.98</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>5.99</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B16">
         <v>2.1</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B17">
         <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B18">
         <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B19">
         <v>2.98</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B20">
         <v>3.66</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B21">
         <v>2.98</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B22">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B23">
         <v>3.98</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B24">
         <v>5.99</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B25">
         <v>5.99</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B26">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B27">
         <v>5.99</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B28">
         <v>1.6</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B29">
         <v>114</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B30">
         <v>118</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B31">
         <v>113.98</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B32">
         <v>117</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B33">
         <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B34">
         <v>158</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B35">
         <v>159</v>
       </c>
       <c r="C35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B36">
         <v>157</v>
       </c>
       <c r="C36" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B37">
         <v>225.3</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B38">
         <v>149</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B39">
         <v>200.02</v>
       </c>
       <c r="C39" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B40">
         <v>289</v>
       </c>
       <c r="C40" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B41">
         <v>289</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B42">
         <v>339.09</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B43">
         <v>765</v>
       </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B44">
         <v>613.64</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B45">
         <v>1047.78</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B46">
         <v>355.5</v>
       </c>
       <c r="C46" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B47">
         <v>425</v>
       </c>
       <c r="C47" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B48">
         <v>460</v>
       </c>
       <c r="C48" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B49">
         <v>445.81</v>
       </c>
       <c r="C49" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B50">
         <v>145</v>
       </c>
       <c r="C50" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B51">
         <v>171.5</v>
       </c>
       <c r="C51" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B52">
         <v>398.95</v>
       </c>
       <c r="C52" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="D10" r:id="rId9"/>
-    <hyperlink ref="D11" r:id="rId10"/>
-    <hyperlink ref="D12" r:id="rId11"/>
-    <hyperlink ref="D13" r:id="rId12"/>
-    <hyperlink ref="D14" r:id="rId13"/>
-    <hyperlink ref="D15" r:id="rId14"/>
-    <hyperlink ref="D16" r:id="rId15"/>
-    <hyperlink ref="D17" r:id="rId16"/>
-    <hyperlink ref="D18" r:id="rId17"/>
-    <hyperlink ref="D19" r:id="rId18"/>
-    <hyperlink ref="D20" r:id="rId19"/>
-    <hyperlink ref="D21" r:id="rId20"/>
-    <hyperlink ref="D22" r:id="rId21"/>
-    <hyperlink ref="D23" r:id="rId22"/>
-    <hyperlink ref="D24" r:id="rId23"/>
-    <hyperlink ref="D25" r:id="rId24"/>
-    <hyperlink ref="D26" r:id="rId25"/>
-    <hyperlink ref="D27" r:id="rId26"/>
-    <hyperlink ref="D28" r:id="rId27"/>
-    <hyperlink ref="D29" r:id="rId28"/>
-    <hyperlink ref="D30" r:id="rId29"/>
-    <hyperlink ref="D31" r:id="rId30"/>
-    <hyperlink ref="D32" r:id="rId31"/>
-    <hyperlink ref="D33" r:id="rId32"/>
-    <hyperlink ref="D34" r:id="rId33"/>
-    <hyperlink ref="D35" r:id="rId34"/>
-    <hyperlink ref="D36" r:id="rId35"/>
-    <hyperlink ref="D37" r:id="rId36"/>
-    <hyperlink ref="D38" r:id="rId37"/>
-    <hyperlink ref="D39" r:id="rId38"/>
-    <hyperlink ref="D40" r:id="rId39"/>
-    <hyperlink ref="D41" r:id="rId40"/>
-    <hyperlink ref="D42" r:id="rId41"/>
-    <hyperlink ref="D43" r:id="rId42"/>
-    <hyperlink ref="D44" r:id="rId43"/>
-    <hyperlink ref="D45" r:id="rId44"/>
-    <hyperlink ref="D46" r:id="rId45"/>
-    <hyperlink ref="D47" r:id="rId46"/>
-    <hyperlink ref="D48" r:id="rId47"/>
-    <hyperlink ref="D49" r:id="rId48"/>
-    <hyperlink ref="D50" r:id="rId49"/>
-    <hyperlink ref="D51" r:id="rId50"/>
-    <hyperlink ref="D52" r:id="rId51"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="D32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="D35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="D36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="D37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="D38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="D40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="D41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="D42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="D43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="D44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="D45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="D46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="D47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="D49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="D50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="D51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="D52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>